<commit_message>
Updated clean - added FB pos
</commit_message>
<xml_diff>
--- a/Dictionary and Notes.xlsx
+++ b/Dictionary and Notes.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick_\Desktop\Learning Fuze\Bootcamp\FF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEF5151-1855-419F-8A0E-D685622F4D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D957BE8-13A5-4037-BECB-8C89E818395F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{6B6C9C32-8EDA-4783-ADAF-78CDB12EB20B}"/>
+    <workbookView xWindow="-19310" yWindow="3480" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{6B6C9C32-8EDA-4783-ADAF-78CDB12EB20B}"/>
   </bookViews>
   <sheets>
     <sheet name="Status Dict" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Stats Dict" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Stats Dict'!$A$3:$C$51</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="182">
   <si>
     <t>status</t>
   </si>
@@ -578,6 +579,15 @@
   </si>
   <si>
     <t>tgt_sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, </t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>games</t>
   </si>
 </sst>
 </file>
@@ -637,16 +647,16 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1216,612 +1226,610 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{443E12E4-49E6-49C1-A30E-AE4F48E3C902}">
   <dimension ref="A2:C84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="2"/>
-    <col min="2" max="2" width="49.25" style="2" customWidth="1"/>
-    <col min="3" max="3" width="220.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.6640625" style="2"/>
+    <col min="2" max="2" width="49.25" customWidth="1"/>
+    <col min="3" max="3" width="220.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3">
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>142</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="A4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="A5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="A6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="A7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="A8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B9" s="5" t="s">
+      <c r="A9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="A10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="A11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="A12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B13" s="5" t="s">
+      <c r="A13" t="s">
+        <v>143</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B14" s="5" t="s">
+      <c r="A14" t="s">
+        <v>143</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B15" s="5" t="s">
+      <c r="A15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B16" s="5" t="s">
+      <c r="A16" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B17" s="5" t="s">
+      <c r="A17" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B18" s="5" t="s">
+      <c r="A18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B19" s="5" t="s">
+      <c r="A19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" t="s">
         <v>144</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B21" s="5" t="s">
+      <c r="A21" t="s">
+        <v>143</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" t="s">
         <v>144</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B23" s="5" t="s">
+      <c r="A23" t="s">
+        <v>143</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="2" t="s">
+      <c r="A24" t="s">
         <v>144</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B25" s="5" t="s">
+      <c r="A25" t="s">
+        <v>143</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B26" s="5" t="s">
+      <c r="A26" t="s">
+        <v>143</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B27" s="5" t="s">
+      <c r="A27" t="s">
+        <v>143</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B28" s="5" t="s">
+      <c r="A28" t="s">
+        <v>143</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B29" s="5" t="s">
+      <c r="A29" t="s">
+        <v>143</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B30" s="5" t="s">
+      <c r="A30" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="2" t="s">
+      <c r="A31" t="s">
         <v>144</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="4" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B32" s="5" t="s">
+      <c r="A32" t="s">
+        <v>143</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="4" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B33" s="5" t="s">
+      <c r="A33" t="s">
+        <v>143</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="4" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B34" s="5" t="s">
+      <c r="A34" t="s">
+        <v>143</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="4" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B35" s="5" t="s">
+      <c r="A35" t="s">
+        <v>143</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B36" s="5" t="s">
+      <c r="A36" t="s">
+        <v>143</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B37" s="5" t="s">
+      <c r="A37" t="s">
+        <v>143</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B38" s="5" t="s">
+      <c r="A38" t="s">
+        <v>143</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="4" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B39" s="5" t="s">
+      <c r="A39" t="s">
+        <v>143</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="4" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B40" s="5" t="s">
+      <c r="A40" t="s">
+        <v>143</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="4" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B41" s="5" t="s">
+      <c r="A41" t="s">
+        <v>143</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="4" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="2" t="s">
+      <c r="A42" t="s">
         <v>144</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="4" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="2" t="s">
+      <c r="A43" t="s">
         <v>144</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="4" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="2" t="s">
+      <c r="A44" t="s">
         <v>144</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="4" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="2" t="s">
+      <c r="A45" t="s">
         <v>144</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="4" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="2" t="s">
+      <c r="A46" t="s">
         <v>144</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="4" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="2" t="s">
+      <c r="A47" t="s">
         <v>144</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="4" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B48" s="5" t="s">
+      <c r="A48" t="s">
+        <v>143</v>
+      </c>
+      <c r="B48" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="4" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B49" s="5" t="s">
+      <c r="A49" t="s">
+        <v>143</v>
+      </c>
+      <c r="B49" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="4" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B50" s="5" t="s">
+      <c r="A50" t="s">
+        <v>143</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C50" s="4" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B51" s="5" t="s">
+      <c r="A51" t="s">
+        <v>143</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C51" s="4" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="B57" s="2" t="s">
+      <c r="B57" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="2" t="str">
+      <c r="C57" t="str">
         <f>_xlfn.CONCAT(B57:B65)</f>
         <v xml:space="preserve">passing_yards_after_catch, passing_epa, dakota, rushing_epa, fantasy_points, fantasy_points_ppr, pacr, racr, receiving_epa </v>
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="B58" s="2" t="s">
+      <c r="B58" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="B59" s="2" t="s">
+      <c r="B59" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="B60" s="2" t="s">
+      <c r="B60" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="B61" s="2" t="s">
+      <c r="B61" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="62" spans="1:3">
-      <c r="B62" s="2" t="s">
+      <c r="B62" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="B63" s="2" t="s">
+      <c r="B63" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="64" spans="1:3">
-      <c r="B64" s="2" t="s">
+      <c r="B64" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="65" spans="1:3">
-      <c r="B65" s="2" t="s">
+      <c r="B65" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="2" t="s">
+      <c r="A73" t="s">
         <v>143</v>
       </c>
       <c r="B73" t="s">
@@ -1832,7 +1840,7 @@
       </c>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="2" t="s">
+      <c r="A74" t="s">
         <v>143</v>
       </c>
       <c r="B74" t="s">
@@ -1843,7 +1851,7 @@
       </c>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="2" t="s">
+      <c r="A75" t="s">
         <v>143</v>
       </c>
       <c r="B75" t="s">
@@ -1854,7 +1862,7 @@
       </c>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" s="2" t="s">
+      <c r="A76" t="s">
         <v>143</v>
       </c>
       <c r="B76" t="s">
@@ -1865,7 +1873,7 @@
       </c>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="2" t="s">
+      <c r="A77" t="s">
         <v>143</v>
       </c>
       <c r="B77" t="s">
@@ -1876,7 +1884,7 @@
       </c>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" s="2" t="s">
+      <c r="A78" t="s">
         <v>143</v>
       </c>
       <c r="B78" t="s">
@@ -1887,7 +1895,7 @@
       </c>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" s="2" t="s">
+      <c r="A79" t="s">
         <v>143</v>
       </c>
       <c r="B79" t="s">
@@ -1898,7 +1906,7 @@
       </c>
     </row>
     <row r="80" spans="1:3">
-      <c r="A80" s="2" t="s">
+      <c r="A80" t="s">
         <v>143</v>
       </c>
       <c r="B80" t="s">
@@ -1909,7 +1917,7 @@
       </c>
     </row>
     <row r="81" spans="1:3">
-      <c r="A81" s="2" t="s">
+      <c r="A81" t="s">
         <v>144</v>
       </c>
       <c r="B81" t="s">
@@ -1920,7 +1928,7 @@
       </c>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="2" t="s">
+      <c r="A82" t="s">
         <v>144</v>
       </c>
       <c r="B82" t="s">
@@ -1931,7 +1939,7 @@
       </c>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="2" t="s">
+      <c r="A83" t="s">
         <v>143</v>
       </c>
       <c r="B83" t="s">
@@ -1942,7 +1950,7 @@
       </c>
     </row>
     <row r="84" spans="1:3">
-      <c r="A84" s="2" t="s">
+      <c r="A84" t="s">
         <v>143</v>
       </c>
       <c r="B84" t="s">
@@ -1961,4 +1969,1179 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F76F7A1-5649-462E-A1EE-A734377ECA77}">
+  <dimension ref="B1:J69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="3" max="4" width="23.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9">
+      <c r="B1" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F1" t="str">
+        <f>_xlfn.CONCAT(B1:E1)</f>
+        <v xml:space="preserve">"completions", </v>
+      </c>
+      <c r="I1" t="str">
+        <f>_xlfn.CONCAT(F1:F31)</f>
+        <v xml:space="preserve">"completions", "attempts", "passing_yards", "passing_tds", "interceptions", "sacks", "sack_yards", "sack_fumbles", "sack_fumbles_lost", "passing_air_yards", "passing_first_downs", "passing_2pt_conversions", "carries", "rushing_yards", "rushing_tds", "rushing_fumbles", "rushing_fumbles_lost", "rushing_first_downs", "rushing_2pt_conversions", "receptions", "targets", "receiving_yards", "receiving_tds", "receiving_fumbles", "receiving_fumbles_lost", "receiving_air_yards", "receiving_yards_after_catch", "receiving_first_downs", "receiving_2pt_conversions", "special_teams_tds", "receiving_2pt_conversions", </v>
+      </c>
+    </row>
+    <row r="2" spans="2:9">
+      <c r="B2" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F2" t="str">
+        <f t="shared" ref="F2:F31" si="0">_xlfn.CONCAT(B2:E2)</f>
+        <v xml:space="preserve">"attempts", </v>
+      </c>
+    </row>
+    <row r="3" spans="2:9">
+      <c r="B3" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"passing_yards", </v>
+      </c>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="B4" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" t="s">
+        <v>180</v>
+      </c>
+      <c r="E4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"passing_tds", </v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>180</v>
+      </c>
+      <c r="E5" t="s">
+        <v>179</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"interceptions", </v>
+      </c>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="B6" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" t="s">
+        <v>180</v>
+      </c>
+      <c r="E6" t="s">
+        <v>179</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"sacks", </v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E7" t="s">
+        <v>179</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"sack_yards", </v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" t="s">
+        <v>180</v>
+      </c>
+      <c r="E8" t="s">
+        <v>179</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"sack_fumbles", </v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" t="s">
+        <v>180</v>
+      </c>
+      <c r="E9" t="s">
+        <v>179</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"sack_fumbles_lost", </v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" t="s">
+        <v>180</v>
+      </c>
+      <c r="E10" t="s">
+        <v>179</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"passing_air_yards", </v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" t="s">
+        <v>180</v>
+      </c>
+      <c r="E11" t="s">
+        <v>179</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"passing_first_downs", </v>
+      </c>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" t="s">
+        <v>180</v>
+      </c>
+      <c r="E12" t="s">
+        <v>179</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"passing_2pt_conversions", </v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" t="s">
+        <v>180</v>
+      </c>
+      <c r="E13" t="s">
+        <v>179</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"carries", </v>
+      </c>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" t="s">
+        <v>180</v>
+      </c>
+      <c r="E14" t="s">
+        <v>179</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"rushing_yards", </v>
+      </c>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" t="s">
+        <v>180</v>
+      </c>
+      <c r="E15" t="s">
+        <v>179</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"rushing_tds", </v>
+      </c>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="B16" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" t="s">
+        <v>180</v>
+      </c>
+      <c r="E16" t="s">
+        <v>179</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"rushing_fumbles", </v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" t="s">
+        <v>180</v>
+      </c>
+      <c r="E17" t="s">
+        <v>179</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"rushing_fumbles_lost", </v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" t="s">
+        <v>180</v>
+      </c>
+      <c r="E18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"rushing_first_downs", </v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" t="s">
+        <v>180</v>
+      </c>
+      <c r="E19" t="s">
+        <v>179</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"rushing_2pt_conversions", </v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" t="s">
+        <v>180</v>
+      </c>
+      <c r="E20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"receptions", </v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C21" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" t="s">
+        <v>180</v>
+      </c>
+      <c r="E21" t="s">
+        <v>179</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"targets", </v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C22" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" t="s">
+        <v>180</v>
+      </c>
+      <c r="E22" t="s">
+        <v>179</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"receiving_yards", </v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C23" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" t="s">
+        <v>180</v>
+      </c>
+      <c r="E23" t="s">
+        <v>179</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"receiving_tds", </v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C24" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" t="s">
+        <v>180</v>
+      </c>
+      <c r="E24" t="s">
+        <v>179</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"receiving_fumbles", </v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C25" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25" t="s">
+        <v>180</v>
+      </c>
+      <c r="E25" t="s">
+        <v>179</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"receiving_fumbles_lost", </v>
+      </c>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C26" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" t="s">
+        <v>180</v>
+      </c>
+      <c r="E26" t="s">
+        <v>179</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"receiving_air_yards", </v>
+      </c>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="B27" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C27" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" t="s">
+        <v>180</v>
+      </c>
+      <c r="E27" t="s">
+        <v>179</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"receiving_yards_after_catch", </v>
+      </c>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="B28" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C28" t="s">
+        <v>134</v>
+      </c>
+      <c r="D28" t="s">
+        <v>180</v>
+      </c>
+      <c r="E28" t="s">
+        <v>179</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"receiving_first_downs", </v>
+      </c>
+    </row>
+    <row r="29" spans="2:6">
+      <c r="B29" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29" t="s">
+        <v>180</v>
+      </c>
+      <c r="E29" t="s">
+        <v>179</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"receiving_2pt_conversions", </v>
+      </c>
+    </row>
+    <row r="30" spans="2:6">
+      <c r="B30" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C30" t="s">
+        <v>136</v>
+      </c>
+      <c r="D30" t="s">
+        <v>180</v>
+      </c>
+      <c r="E30" t="s">
+        <v>179</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"special_teams_tds", </v>
+      </c>
+    </row>
+    <row r="31" spans="2:6">
+      <c r="B31" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C31" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31" t="s">
+        <v>180</v>
+      </c>
+      <c r="E31" t="s">
+        <v>179</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"receiving_2pt_conversions", </v>
+      </c>
+    </row>
+    <row r="32" spans="2:6">
+      <c r="B32" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C32" t="s">
+        <v>136</v>
+      </c>
+      <c r="D32" t="s">
+        <v>180</v>
+      </c>
+      <c r="E32" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="38" spans="3:10">
+      <c r="C38" t="s">
+        <v>180</v>
+      </c>
+      <c r="D38" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38" t="s">
+        <v>180</v>
+      </c>
+      <c r="F38" t="s">
+        <v>179</v>
+      </c>
+      <c r="G38" t="str">
+        <f>_xlfn.CONCAT(C38:F38)</f>
+        <v xml:space="preserve">"season_type", </v>
+      </c>
+      <c r="J38" t="str">
+        <f>_xlfn.CONCAT(G38:G69)</f>
+        <v xml:space="preserve">"season_type", "completions", "attempts", "passing_yards", "passing_tds", "interceptions", "sacks", "sack_yards", "sack_fumbles", "sack_fumbles_lost", "passing_air_yards", "passing_first_downs", "passing_2pt_conversions", "carries", "rushing_yards", "rushing_tds", "rushing_fumbles", "rushing_fumbles_lost", "rushing_first_downs", "rushing_2pt_conversions", "receptions", "targets", "receiving_yards", "receiving_tds", "receiving_fumbles", "receiving_fumbles_lost", "receiving_air_yards", "receiving_yards_after_catch", "receiving_first_downs", "receiving_2pt_conversions", "special_teams_tds", "games", </v>
+      </c>
+    </row>
+    <row r="39" spans="3:10">
+      <c r="C39" t="s">
+        <v>180</v>
+      </c>
+      <c r="D39" t="s">
+        <v>58</v>
+      </c>
+      <c r="E39" t="s">
+        <v>180</v>
+      </c>
+      <c r="F39" t="s">
+        <v>179</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" ref="G39:G69" si="1">_xlfn.CONCAT(C39:F39)</f>
+        <v xml:space="preserve">"completions", </v>
+      </c>
+    </row>
+    <row r="40" spans="3:10">
+      <c r="C40" t="s">
+        <v>180</v>
+      </c>
+      <c r="D40" t="s">
+        <v>60</v>
+      </c>
+      <c r="E40" t="s">
+        <v>180</v>
+      </c>
+      <c r="F40" t="s">
+        <v>179</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"attempts", </v>
+      </c>
+    </row>
+    <row r="41" spans="3:10">
+      <c r="C41" t="s">
+        <v>180</v>
+      </c>
+      <c r="D41" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" t="s">
+        <v>180</v>
+      </c>
+      <c r="F41" t="s">
+        <v>179</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"passing_yards", </v>
+      </c>
+    </row>
+    <row r="42" spans="3:10">
+      <c r="C42" t="s">
+        <v>180</v>
+      </c>
+      <c r="D42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E42" t="s">
+        <v>180</v>
+      </c>
+      <c r="F42" t="s">
+        <v>179</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"passing_tds", </v>
+      </c>
+    </row>
+    <row r="43" spans="3:10">
+      <c r="C43" t="s">
+        <v>180</v>
+      </c>
+      <c r="D43" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43" t="s">
+        <v>180</v>
+      </c>
+      <c r="F43" t="s">
+        <v>179</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"interceptions", </v>
+      </c>
+    </row>
+    <row r="44" spans="3:10">
+      <c r="C44" t="s">
+        <v>180</v>
+      </c>
+      <c r="D44" t="s">
+        <v>68</v>
+      </c>
+      <c r="E44" t="s">
+        <v>180</v>
+      </c>
+      <c r="F44" t="s">
+        <v>179</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"sacks", </v>
+      </c>
+    </row>
+    <row r="45" spans="3:10">
+      <c r="C45" t="s">
+        <v>180</v>
+      </c>
+      <c r="D45" t="s">
+        <v>70</v>
+      </c>
+      <c r="E45" t="s">
+        <v>180</v>
+      </c>
+      <c r="F45" t="s">
+        <v>179</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"sack_yards", </v>
+      </c>
+    </row>
+    <row r="46" spans="3:10">
+      <c r="C46" t="s">
+        <v>180</v>
+      </c>
+      <c r="D46" t="s">
+        <v>72</v>
+      </c>
+      <c r="E46" t="s">
+        <v>180</v>
+      </c>
+      <c r="F46" t="s">
+        <v>179</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"sack_fumbles", </v>
+      </c>
+    </row>
+    <row r="47" spans="3:10">
+      <c r="C47" t="s">
+        <v>180</v>
+      </c>
+      <c r="D47" t="s">
+        <v>74</v>
+      </c>
+      <c r="E47" t="s">
+        <v>180</v>
+      </c>
+      <c r="F47" t="s">
+        <v>179</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"sack_fumbles_lost", </v>
+      </c>
+    </row>
+    <row r="48" spans="3:10">
+      <c r="C48" t="s">
+        <v>180</v>
+      </c>
+      <c r="D48" t="s">
+        <v>76</v>
+      </c>
+      <c r="E48" t="s">
+        <v>180</v>
+      </c>
+      <c r="F48" t="s">
+        <v>179</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"passing_air_yards", </v>
+      </c>
+    </row>
+    <row r="49" spans="3:7">
+      <c r="C49" t="s">
+        <v>180</v>
+      </c>
+      <c r="D49" t="s">
+        <v>80</v>
+      </c>
+      <c r="E49" t="s">
+        <v>180</v>
+      </c>
+      <c r="F49" t="s">
+        <v>179</v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"passing_first_downs", </v>
+      </c>
+    </row>
+    <row r="50" spans="3:7">
+      <c r="C50" t="s">
+        <v>180</v>
+      </c>
+      <c r="D50" t="s">
+        <v>84</v>
+      </c>
+      <c r="E50" t="s">
+        <v>180</v>
+      </c>
+      <c r="F50" t="s">
+        <v>179</v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"passing_2pt_conversions", </v>
+      </c>
+    </row>
+    <row r="51" spans="3:7">
+      <c r="C51" t="s">
+        <v>180</v>
+      </c>
+      <c r="D51" t="s">
+        <v>88</v>
+      </c>
+      <c r="E51" t="s">
+        <v>180</v>
+      </c>
+      <c r="F51" t="s">
+        <v>179</v>
+      </c>
+      <c r="G51" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"carries", </v>
+      </c>
+    </row>
+    <row r="52" spans="3:7">
+      <c r="C52" t="s">
+        <v>180</v>
+      </c>
+      <c r="D52" t="s">
+        <v>90</v>
+      </c>
+      <c r="E52" t="s">
+        <v>180</v>
+      </c>
+      <c r="F52" t="s">
+        <v>179</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"rushing_yards", </v>
+      </c>
+    </row>
+    <row r="53" spans="3:7">
+      <c r="C53" t="s">
+        <v>180</v>
+      </c>
+      <c r="D53" t="s">
+        <v>92</v>
+      </c>
+      <c r="E53" t="s">
+        <v>180</v>
+      </c>
+      <c r="F53" t="s">
+        <v>179</v>
+      </c>
+      <c r="G53" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"rushing_tds", </v>
+      </c>
+    </row>
+    <row r="54" spans="3:7">
+      <c r="C54" t="s">
+        <v>180</v>
+      </c>
+      <c r="D54" t="s">
+        <v>94</v>
+      </c>
+      <c r="E54" t="s">
+        <v>180</v>
+      </c>
+      <c r="F54" t="s">
+        <v>179</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"rushing_fumbles", </v>
+      </c>
+    </row>
+    <row r="55" spans="3:7">
+      <c r="C55" t="s">
+        <v>180</v>
+      </c>
+      <c r="D55" t="s">
+        <v>96</v>
+      </c>
+      <c r="E55" t="s">
+        <v>180</v>
+      </c>
+      <c r="F55" t="s">
+        <v>179</v>
+      </c>
+      <c r="G55" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"rushing_fumbles_lost", </v>
+      </c>
+    </row>
+    <row r="56" spans="3:7">
+      <c r="C56" t="s">
+        <v>180</v>
+      </c>
+      <c r="D56" t="s">
+        <v>98</v>
+      </c>
+      <c r="E56" t="s">
+        <v>180</v>
+      </c>
+      <c r="F56" t="s">
+        <v>179</v>
+      </c>
+      <c r="G56" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"rushing_first_downs", </v>
+      </c>
+    </row>
+    <row r="57" spans="3:7">
+      <c r="C57" t="s">
+        <v>180</v>
+      </c>
+      <c r="D57" t="s">
+        <v>102</v>
+      </c>
+      <c r="E57" t="s">
+        <v>180</v>
+      </c>
+      <c r="F57" t="s">
+        <v>179</v>
+      </c>
+      <c r="G57" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"rushing_2pt_conversions", </v>
+      </c>
+    </row>
+    <row r="58" spans="3:7">
+      <c r="C58" t="s">
+        <v>180</v>
+      </c>
+      <c r="D58" t="s">
+        <v>104</v>
+      </c>
+      <c r="E58" t="s">
+        <v>180</v>
+      </c>
+      <c r="F58" t="s">
+        <v>179</v>
+      </c>
+      <c r="G58" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"receptions", </v>
+      </c>
+    </row>
+    <row r="59" spans="3:7">
+      <c r="C59" t="s">
+        <v>180</v>
+      </c>
+      <c r="D59" t="s">
+        <v>106</v>
+      </c>
+      <c r="E59" t="s">
+        <v>180</v>
+      </c>
+      <c r="F59" t="s">
+        <v>179</v>
+      </c>
+      <c r="G59" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"targets", </v>
+      </c>
+    </row>
+    <row r="60" spans="3:7">
+      <c r="C60" t="s">
+        <v>180</v>
+      </c>
+      <c r="D60" t="s">
+        <v>108</v>
+      </c>
+      <c r="E60" t="s">
+        <v>180</v>
+      </c>
+      <c r="F60" t="s">
+        <v>179</v>
+      </c>
+      <c r="G60" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"receiving_yards", </v>
+      </c>
+    </row>
+    <row r="61" spans="3:7">
+      <c r="C61" t="s">
+        <v>180</v>
+      </c>
+      <c r="D61" t="s">
+        <v>110</v>
+      </c>
+      <c r="E61" t="s">
+        <v>180</v>
+      </c>
+      <c r="F61" t="s">
+        <v>179</v>
+      </c>
+      <c r="G61" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"receiving_tds", </v>
+      </c>
+    </row>
+    <row r="62" spans="3:7">
+      <c r="C62" t="s">
+        <v>180</v>
+      </c>
+      <c r="D62" t="s">
+        <v>116</v>
+      </c>
+      <c r="E62" t="s">
+        <v>180</v>
+      </c>
+      <c r="F62" t="s">
+        <v>179</v>
+      </c>
+      <c r="G62" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"receiving_fumbles", </v>
+      </c>
+    </row>
+    <row r="63" spans="3:7">
+      <c r="C63" t="s">
+        <v>180</v>
+      </c>
+      <c r="D63" t="s">
+        <v>118</v>
+      </c>
+      <c r="E63" t="s">
+        <v>180</v>
+      </c>
+      <c r="F63" t="s">
+        <v>179</v>
+      </c>
+      <c r="G63" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"receiving_fumbles_lost", </v>
+      </c>
+    </row>
+    <row r="64" spans="3:7">
+      <c r="C64" t="s">
+        <v>180</v>
+      </c>
+      <c r="D64" t="s">
+        <v>112</v>
+      </c>
+      <c r="E64" t="s">
+        <v>180</v>
+      </c>
+      <c r="F64" t="s">
+        <v>179</v>
+      </c>
+      <c r="G64" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"receiving_air_yards", </v>
+      </c>
+    </row>
+    <row r="65" spans="3:7">
+      <c r="C65" t="s">
+        <v>180</v>
+      </c>
+      <c r="D65" t="s">
+        <v>114</v>
+      </c>
+      <c r="E65" t="s">
+        <v>180</v>
+      </c>
+      <c r="F65" t="s">
+        <v>179</v>
+      </c>
+      <c r="G65" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"receiving_yards_after_catch", </v>
+      </c>
+    </row>
+    <row r="66" spans="3:7">
+      <c r="C66" t="s">
+        <v>180</v>
+      </c>
+      <c r="D66" t="s">
+        <v>134</v>
+      </c>
+      <c r="E66" t="s">
+        <v>180</v>
+      </c>
+      <c r="F66" t="s">
+        <v>179</v>
+      </c>
+      <c r="G66" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"receiving_first_downs", </v>
+      </c>
+    </row>
+    <row r="67" spans="3:7">
+      <c r="C67" t="s">
+        <v>180</v>
+      </c>
+      <c r="D67" t="s">
+        <v>120</v>
+      </c>
+      <c r="E67" t="s">
+        <v>180</v>
+      </c>
+      <c r="F67" t="s">
+        <v>179</v>
+      </c>
+      <c r="G67" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"receiving_2pt_conversions", </v>
+      </c>
+    </row>
+    <row r="68" spans="3:7">
+      <c r="C68" t="s">
+        <v>180</v>
+      </c>
+      <c r="D68" t="s">
+        <v>136</v>
+      </c>
+      <c r="E68" t="s">
+        <v>180</v>
+      </c>
+      <c r="F68" t="s">
+        <v>179</v>
+      </c>
+      <c r="G68" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"special_teams_tds", </v>
+      </c>
+    </row>
+    <row r="69" spans="3:7">
+      <c r="C69" t="s">
+        <v>180</v>
+      </c>
+      <c r="D69" t="s">
+        <v>181</v>
+      </c>
+      <c r="E69" t="s">
+        <v>180</v>
+      </c>
+      <c r="F69" t="s">
+        <v>179</v>
+      </c>
+      <c r="G69" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"games", </v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>